<commit_message>
fix: :card_file_box: FIX DATA 2016
</commit_message>
<xml_diff>
--- a/apps/load_data/2016/01/PLMOVMAE.xlsx
+++ b/apps/load_data/2016/01/PLMOVMAE.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NOMBRADOS -2016\HHY0116\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ACTUALIZADOS\2016\HHY0116\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{52FA05E5-9240-4A0A-9AFF-83CB1336CD6F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8574F8CC-3CEC-4BCD-B2C6-0F1AE3370766}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="10305"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="10305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLMOVMAE" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PLMOVMAE!$A$1:$CF$277</definedName>
     <definedName name="_xlnm.Database">PLMOVMAE!$A$1:$CF$277</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10281" uniqueCount="2726">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10267" uniqueCount="2725">
   <si>
     <t>CODEJE</t>
   </si>
@@ -7226,9 +7227,6 @@
   </si>
   <si>
     <t>0143A         1</t>
-  </si>
-  <si>
-    <t>S/N</t>
   </si>
   <si>
     <t>1081    296920    2969201082    159880    1598802001         0     386002006     22500     225002026    158280    1582802086      2500      25002180       250       2502182       100       1002503        50        503004         0     26723</t>
@@ -8206,7 +8204,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -9046,10 +9044,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CF277"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AB281" sqref="AB281"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -49176,12 +49176,7 @@
       <c r="AA244" s="1">
         <v>0</v>
       </c>
-      <c r="AC244" s="3">
-        <v>42309</v>
-      </c>
-      <c r="AD244" s="1" t="s">
-        <v>2401</v>
-      </c>
+      <c r="AC244" s="3"/>
       <c r="AF244" s="1" t="s">
         <v>103</v>
       </c>
@@ -49240,7 +49235,7 @@
         <v>110</v>
       </c>
       <c r="BH244" s="1" t="s">
-        <v>2402</v>
+        <v>2401</v>
       </c>
       <c r="BI244" s="1" t="s">
         <v>2070</v>
@@ -49252,7 +49247,7 @@
         <v>102</v>
       </c>
       <c r="BT244" s="1" t="s">
-        <v>2403</v>
+        <v>2402</v>
       </c>
       <c r="BU244" s="1" t="s">
         <v>117</v>
@@ -49273,13 +49268,13 @@
         <v>108</v>
       </c>
       <c r="CC244" s="1" t="s">
+        <v>2403</v>
+      </c>
+      <c r="CD244" s="1" t="s">
         <v>2404</v>
       </c>
-      <c r="CD244" s="1" t="s">
+      <c r="CE244" s="1" t="s">
         <v>2405</v>
-      </c>
-      <c r="CE244" s="1" t="s">
-        <v>2406</v>
       </c>
     </row>
     <row r="245" spans="1:83" x14ac:dyDescent="0.25">
@@ -49314,19 +49309,19 @@
         <v>93</v>
       </c>
       <c r="K245" s="1" t="s">
+        <v>2406</v>
+      </c>
+      <c r="L245" s="1" t="s">
         <v>2407</v>
       </c>
-      <c r="L245" s="1" t="s">
+      <c r="N245" s="1" t="s">
         <v>2408</v>
-      </c>
-      <c r="N245" s="1" t="s">
-        <v>2409</v>
       </c>
       <c r="O245" s="1" t="s">
         <v>97</v>
       </c>
       <c r="P245" s="1" t="s">
-        <v>2410</v>
+        <v>2409</v>
       </c>
       <c r="Q245" s="3">
         <v>27241</v>
@@ -49352,12 +49347,7 @@
       <c r="AB245" s="1" t="s">
         <v>584</v>
       </c>
-      <c r="AC245" s="3">
-        <v>42309</v>
-      </c>
-      <c r="AD245" s="1" t="s">
-        <v>2401</v>
-      </c>
+      <c r="AC245" s="3"/>
       <c r="AF245" s="1" t="s">
         <v>103</v>
       </c>
@@ -49404,7 +49394,7 @@
         <v>108</v>
       </c>
       <c r="AZ245" s="1" t="s">
-        <v>2411</v>
+        <v>2410</v>
       </c>
       <c r="BB245" s="1">
         <v>1</v>
@@ -49416,7 +49406,7 @@
         <v>110</v>
       </c>
       <c r="BH245" s="1" t="s">
-        <v>2412</v>
+        <v>2411</v>
       </c>
       <c r="BI245" s="1" t="s">
         <v>1666</v>
@@ -49431,13 +49421,13 @@
         <v>99</v>
       </c>
       <c r="BR245" s="1" t="s">
-        <v>2413</v>
+        <v>2412</v>
       </c>
       <c r="BS245" s="3">
         <v>36949</v>
       </c>
       <c r="BT245" s="1" t="s">
-        <v>2414</v>
+        <v>2413</v>
       </c>
       <c r="BU245" s="1" t="s">
         <v>117</v>
@@ -49461,13 +49451,13 @@
         <v>108</v>
       </c>
       <c r="CC245" s="1" t="s">
-        <v>2415</v>
+        <v>2414</v>
       </c>
       <c r="CD245" s="1" t="s">
         <v>1960</v>
       </c>
       <c r="CE245" s="1" t="s">
-        <v>2416</v>
+        <v>2415</v>
       </c>
     </row>
     <row r="246" spans="1:83" x14ac:dyDescent="0.25">
@@ -49502,19 +49492,19 @@
         <v>93</v>
       </c>
       <c r="K246" s="1" t="s">
+        <v>2416</v>
+      </c>
+      <c r="L246" s="1" t="s">
         <v>2417</v>
       </c>
-      <c r="L246" s="1" t="s">
+      <c r="N246" s="1" t="s">
         <v>2418</v>
-      </c>
-      <c r="N246" s="1" t="s">
-        <v>2419</v>
       </c>
       <c r="O246" s="1" t="s">
         <v>97</v>
       </c>
       <c r="P246" s="1" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
       <c r="Q246" s="3">
         <v>25223</v>
@@ -49540,12 +49530,7 @@
       <c r="AB246" s="1" t="s">
         <v>584</v>
       </c>
-      <c r="AC246" s="3">
-        <v>42309</v>
-      </c>
-      <c r="AD246" s="1" t="s">
-        <v>2401</v>
-      </c>
+      <c r="AC246" s="3"/>
       <c r="AF246" s="1" t="s">
         <v>103</v>
       </c>
@@ -49592,7 +49577,7 @@
         <v>108</v>
       </c>
       <c r="AZ246" s="1" t="s">
-        <v>2421</v>
+        <v>2420</v>
       </c>
       <c r="BB246" s="1">
         <v>1</v>
@@ -49607,10 +49592,10 @@
         <v>110</v>
       </c>
       <c r="BH246" s="1" t="s">
+        <v>2421</v>
+      </c>
+      <c r="BI246" s="1" t="s">
         <v>2422</v>
-      </c>
-      <c r="BI246" s="1" t="s">
-        <v>2423</v>
       </c>
       <c r="BM246" s="1" t="s">
         <v>113</v>
@@ -49622,13 +49607,13 @@
         <v>99</v>
       </c>
       <c r="BR246" s="1" t="s">
-        <v>2424</v>
+        <v>2423</v>
       </c>
       <c r="BS246" s="3">
         <v>36825</v>
       </c>
       <c r="BT246" s="1" t="s">
-        <v>2425</v>
+        <v>2424</v>
       </c>
       <c r="BU246" s="1" t="s">
         <v>117</v>
@@ -49652,13 +49637,13 @@
         <v>108</v>
       </c>
       <c r="CC246" s="1" t="s">
+        <v>2425</v>
+      </c>
+      <c r="CD246" s="1" t="s">
         <v>2426</v>
       </c>
-      <c r="CD246" s="1" t="s">
+      <c r="CE246" s="1" t="s">
         <v>2427</v>
-      </c>
-      <c r="CE246" s="1" t="s">
-        <v>2428</v>
       </c>
     </row>
     <row r="247" spans="1:83" x14ac:dyDescent="0.25">
@@ -49693,19 +49678,19 @@
         <v>93</v>
       </c>
       <c r="K247" s="1" t="s">
+        <v>2428</v>
+      </c>
+      <c r="L247" s="1" t="s">
         <v>2429</v>
       </c>
-      <c r="L247" s="1" t="s">
+      <c r="N247" s="1" t="s">
         <v>2430</v>
-      </c>
-      <c r="N247" s="1" t="s">
-        <v>2431</v>
       </c>
       <c r="O247" s="1" t="s">
         <v>97</v>
       </c>
       <c r="P247" s="1" t="s">
-        <v>2432</v>
+        <v>2431</v>
       </c>
       <c r="Q247" s="3">
         <v>27018</v>
@@ -49728,12 +49713,7 @@
       <c r="AA247" s="1">
         <v>0</v>
       </c>
-      <c r="AC247" s="3">
-        <v>42309</v>
-      </c>
-      <c r="AD247" s="1" t="s">
-        <v>2401</v>
-      </c>
+      <c r="AC247" s="3"/>
       <c r="AF247" s="1" t="s">
         <v>103</v>
       </c>
@@ -49783,7 +49763,7 @@
         <v>108</v>
       </c>
       <c r="AZ247" s="1" t="s">
-        <v>2433</v>
+        <v>2432</v>
       </c>
       <c r="BB247" s="1">
         <v>1</v>
@@ -49795,7 +49775,7 @@
         <v>110</v>
       </c>
       <c r="BH247" s="1" t="s">
-        <v>2434</v>
+        <v>2433</v>
       </c>
       <c r="BI247" s="1" t="s">
         <v>192</v>
@@ -49807,7 +49787,7 @@
         <v>102</v>
       </c>
       <c r="BT247" s="1" t="s">
-        <v>2435</v>
+        <v>2434</v>
       </c>
       <c r="BU247" s="1" t="s">
         <v>117</v>
@@ -49825,13 +49805,13 @@
         <v>108</v>
       </c>
       <c r="CC247" s="1" t="s">
-        <v>2436</v>
+        <v>2435</v>
       </c>
       <c r="CD247" s="1" t="s">
         <v>1231</v>
       </c>
       <c r="CE247" s="1" t="s">
-        <v>2437</v>
+        <v>2436</v>
       </c>
     </row>
     <row r="248" spans="1:83" x14ac:dyDescent="0.25">
@@ -49866,19 +49846,19 @@
         <v>93</v>
       </c>
       <c r="K248" s="1" t="s">
+        <v>2437</v>
+      </c>
+      <c r="L248" s="1" t="s">
         <v>2438</v>
       </c>
-      <c r="L248" s="1" t="s">
+      <c r="N248" s="1" t="s">
         <v>2439</v>
-      </c>
-      <c r="N248" s="1" t="s">
-        <v>2440</v>
       </c>
       <c r="O248" s="1" t="s">
         <v>97</v>
       </c>
       <c r="P248" s="1" t="s">
-        <v>2441</v>
+        <v>2440</v>
       </c>
       <c r="Q248" s="3">
         <v>29037</v>
@@ -49901,12 +49881,7 @@
       <c r="AA248" s="1">
         <v>0</v>
       </c>
-      <c r="AC248" s="3">
-        <v>42309</v>
-      </c>
-      <c r="AD248" s="1" t="s">
-        <v>2401</v>
-      </c>
+      <c r="AC248" s="3"/>
       <c r="AF248" s="1" t="s">
         <v>103</v>
       </c>
@@ -49956,7 +49931,7 @@
         <v>108</v>
       </c>
       <c r="AZ248" s="1" t="s">
-        <v>2442</v>
+        <v>2441</v>
       </c>
       <c r="BB248" s="1">
         <v>1</v>
@@ -49968,7 +49943,7 @@
         <v>110</v>
       </c>
       <c r="BH248" s="1" t="s">
-        <v>2443</v>
+        <v>2442</v>
       </c>
       <c r="BM248" s="1" t="s">
         <v>113</v>
@@ -49977,7 +49952,7 @@
         <v>102</v>
       </c>
       <c r="BT248" s="1" t="s">
-        <v>2444</v>
+        <v>2443</v>
       </c>
       <c r="BU248" s="1" t="s">
         <v>117</v>
@@ -49998,10 +49973,10 @@
         <v>712</v>
       </c>
       <c r="CD248" s="1" t="s">
+        <v>2444</v>
+      </c>
+      <c r="CE248" s="1" t="s">
         <v>2445</v>
-      </c>
-      <c r="CE248" s="1" t="s">
-        <v>2446</v>
       </c>
     </row>
     <row r="249" spans="1:83" x14ac:dyDescent="0.25">
@@ -50036,19 +50011,19 @@
         <v>93</v>
       </c>
       <c r="K249" s="1" t="s">
+        <v>2446</v>
+      </c>
+      <c r="L249" s="1" t="s">
         <v>2447</v>
       </c>
-      <c r="L249" s="1" t="s">
+      <c r="N249" s="1" t="s">
         <v>2448</v>
-      </c>
-      <c r="N249" s="1" t="s">
-        <v>2449</v>
       </c>
       <c r="O249" s="1" t="s">
         <v>97</v>
       </c>
       <c r="P249" s="1" t="s">
-        <v>2450</v>
+        <v>2449</v>
       </c>
       <c r="Q249" s="3">
         <v>26647</v>
@@ -50071,12 +50046,7 @@
       <c r="AA249" s="1">
         <v>0</v>
       </c>
-      <c r="AC249" s="3">
-        <v>42309</v>
-      </c>
-      <c r="AD249" s="1" t="s">
-        <v>2401</v>
-      </c>
+      <c r="AC249" s="3"/>
       <c r="AF249" s="1" t="s">
         <v>103</v>
       </c>
@@ -50126,7 +50096,7 @@
         <v>108</v>
       </c>
       <c r="AZ249" s="1" t="s">
-        <v>2451</v>
+        <v>2450</v>
       </c>
       <c r="BB249" s="1">
         <v>1</v>
@@ -50138,7 +50108,7 @@
         <v>110</v>
       </c>
       <c r="BH249" s="1" t="s">
-        <v>2452</v>
+        <v>2451</v>
       </c>
       <c r="BI249" s="1" t="s">
         <v>192</v>
@@ -50150,7 +50120,7 @@
         <v>102</v>
       </c>
       <c r="BT249" s="1" t="s">
-        <v>2453</v>
+        <v>2452</v>
       </c>
       <c r="BU249" s="1" t="s">
         <v>117</v>
@@ -50168,13 +50138,13 @@
         <v>108</v>
       </c>
       <c r="CC249" s="1" t="s">
+        <v>2453</v>
+      </c>
+      <c r="CD249" s="1" t="s">
+        <v>2453</v>
+      </c>
+      <c r="CE249" s="1" t="s">
         <v>2454</v>
-      </c>
-      <c r="CD249" s="1" t="s">
-        <v>2454</v>
-      </c>
-      <c r="CE249" s="1" t="s">
-        <v>2455</v>
       </c>
     </row>
     <row r="250" spans="1:83" x14ac:dyDescent="0.25">
@@ -50209,19 +50179,19 @@
         <v>93</v>
       </c>
       <c r="K250" s="1" t="s">
+        <v>2455</v>
+      </c>
+      <c r="L250" s="1" t="s">
         <v>2456</v>
       </c>
-      <c r="L250" s="1" t="s">
+      <c r="N250" s="1" t="s">
         <v>2457</v>
-      </c>
-      <c r="N250" s="1" t="s">
-        <v>2458</v>
       </c>
       <c r="O250" s="1" t="s">
         <v>97</v>
       </c>
       <c r="P250" s="1" t="s">
-        <v>2459</v>
+        <v>2458</v>
       </c>
       <c r="Q250" s="3">
         <v>25405</v>
@@ -50250,12 +50220,7 @@
       <c r="AA250" s="1">
         <v>0</v>
       </c>
-      <c r="AC250" s="3">
-        <v>42309</v>
-      </c>
-      <c r="AD250" s="1" t="s">
-        <v>2401</v>
-      </c>
+      <c r="AC250" s="3"/>
       <c r="AF250" s="1" t="s">
         <v>103</v>
       </c>
@@ -50302,7 +50267,7 @@
         <v>108</v>
       </c>
       <c r="AZ250" s="1" t="s">
-        <v>2460</v>
+        <v>2459</v>
       </c>
       <c r="BB250" s="1">
         <v>1</v>
@@ -50317,7 +50282,7 @@
         <v>110</v>
       </c>
       <c r="BH250" s="1" t="s">
-        <v>2461</v>
+        <v>2460</v>
       </c>
       <c r="BI250" s="1" t="s">
         <v>452</v>
@@ -50332,13 +50297,13 @@
         <v>114</v>
       </c>
       <c r="BR250" s="1" t="s">
-        <v>2462</v>
+        <v>2461</v>
       </c>
       <c r="BS250" s="3">
         <v>35243</v>
       </c>
       <c r="BT250" s="1" t="s">
-        <v>2463</v>
+        <v>2462</v>
       </c>
       <c r="BU250" s="1" t="s">
         <v>117</v>
@@ -50356,13 +50321,13 @@
         <v>108</v>
       </c>
       <c r="CC250" s="1" t="s">
+        <v>2463</v>
+      </c>
+      <c r="CD250" s="1" t="s">
         <v>2464</v>
       </c>
-      <c r="CD250" s="1" t="s">
+      <c r="CE250" s="1" t="s">
         <v>2465</v>
-      </c>
-      <c r="CE250" s="1" t="s">
-        <v>2466</v>
       </c>
     </row>
     <row r="251" spans="1:83" x14ac:dyDescent="0.25">
@@ -50397,19 +50362,19 @@
         <v>93</v>
       </c>
       <c r="K251" s="1" t="s">
+        <v>2466</v>
+      </c>
+      <c r="L251" s="1" t="s">
         <v>2467</v>
       </c>
-      <c r="L251" s="1" t="s">
+      <c r="N251" s="1" t="s">
         <v>2468</v>
-      </c>
-      <c r="N251" s="1" t="s">
-        <v>2469</v>
       </c>
       <c r="O251" s="1" t="s">
         <v>97</v>
       </c>
       <c r="P251" s="1" t="s">
-        <v>2470</v>
+        <v>2469</v>
       </c>
       <c r="Q251" s="3">
         <v>28845</v>
@@ -50432,12 +50397,7 @@
       <c r="AA251" s="1">
         <v>0</v>
       </c>
-      <c r="AC251" s="3">
-        <v>42309</v>
-      </c>
-      <c r="AD251" s="1" t="s">
-        <v>2401</v>
-      </c>
+      <c r="AC251" s="3"/>
       <c r="AF251" s="1" t="s">
         <v>103</v>
       </c>
@@ -50487,7 +50447,7 @@
         <v>108</v>
       </c>
       <c r="AZ251" s="1" t="s">
-        <v>2471</v>
+        <v>2470</v>
       </c>
       <c r="BB251" s="1">
         <v>1</v>
@@ -50499,7 +50459,7 @@
         <v>110</v>
       </c>
       <c r="BH251" s="1" t="s">
-        <v>2472</v>
+        <v>2471</v>
       </c>
       <c r="BI251" s="1" t="s">
         <v>192</v>
@@ -50511,7 +50471,7 @@
         <v>102</v>
       </c>
       <c r="BT251" s="1" t="s">
-        <v>2473</v>
+        <v>2472</v>
       </c>
       <c r="BU251" s="1" t="s">
         <v>117</v>
@@ -50529,13 +50489,13 @@
         <v>108</v>
       </c>
       <c r="CC251" s="1" t="s">
+        <v>2473</v>
+      </c>
+      <c r="CD251" s="1" t="s">
         <v>2474</v>
       </c>
-      <c r="CD251" s="1" t="s">
+      <c r="CE251" s="1" t="s">
         <v>2475</v>
-      </c>
-      <c r="CE251" s="1" t="s">
-        <v>2476</v>
       </c>
     </row>
     <row r="252" spans="1:83" x14ac:dyDescent="0.25">
@@ -50570,19 +50530,19 @@
         <v>93</v>
       </c>
       <c r="K252" s="1" t="s">
+        <v>2476</v>
+      </c>
+      <c r="L252" s="1" t="s">
         <v>2477</v>
       </c>
-      <c r="L252" s="1" t="s">
+      <c r="N252" s="1" t="s">
         <v>2478</v>
-      </c>
-      <c r="N252" s="1" t="s">
-        <v>2479</v>
       </c>
       <c r="O252" s="1" t="s">
         <v>97</v>
       </c>
       <c r="P252" s="1" t="s">
-        <v>2480</v>
+        <v>2479</v>
       </c>
       <c r="Q252" s="3">
         <v>21425</v>
@@ -50605,12 +50565,7 @@
       <c r="AA252" s="1">
         <v>0</v>
       </c>
-      <c r="AC252" s="3">
-        <v>42309</v>
-      </c>
-      <c r="AD252" s="1" t="s">
-        <v>2401</v>
-      </c>
+      <c r="AC252" s="3"/>
       <c r="AF252" s="1" t="s">
         <v>103</v>
       </c>
@@ -50660,7 +50615,7 @@
         <v>108</v>
       </c>
       <c r="AZ252" s="1" t="s">
-        <v>2481</v>
+        <v>2480</v>
       </c>
       <c r="BB252" s="1">
         <v>1</v>
@@ -50672,10 +50627,10 @@
         <v>110</v>
       </c>
       <c r="BH252" s="1" t="s">
+        <v>2481</v>
+      </c>
+      <c r="BI252" s="1" t="s">
         <v>2482</v>
-      </c>
-      <c r="BI252" s="1" t="s">
-        <v>2483</v>
       </c>
       <c r="BM252" s="1" t="s">
         <v>113</v>
@@ -50684,7 +50639,7 @@
         <v>102</v>
       </c>
       <c r="BT252" s="1" t="s">
-        <v>2484</v>
+        <v>2483</v>
       </c>
       <c r="BU252" s="1" t="s">
         <v>117</v>
@@ -50702,13 +50657,13 @@
         <v>108</v>
       </c>
       <c r="CC252" s="1" t="s">
+        <v>2484</v>
+      </c>
+      <c r="CD252" s="1" t="s">
         <v>2485</v>
       </c>
-      <c r="CD252" s="1" t="s">
+      <c r="CE252" s="1" t="s">
         <v>2486</v>
-      </c>
-      <c r="CE252" s="1" t="s">
-        <v>2487</v>
       </c>
     </row>
     <row r="253" spans="1:83" x14ac:dyDescent="0.25">
@@ -50743,19 +50698,19 @@
         <v>93</v>
       </c>
       <c r="K253" s="1" t="s">
+        <v>2487</v>
+      </c>
+      <c r="L253" s="1" t="s">
         <v>2488</v>
       </c>
-      <c r="L253" s="1" t="s">
+      <c r="N253" s="1" t="s">
         <v>2489</v>
-      </c>
-      <c r="N253" s="1" t="s">
-        <v>2490</v>
       </c>
       <c r="O253" s="1" t="s">
         <v>97</v>
       </c>
       <c r="P253" s="1" t="s">
-        <v>2491</v>
+        <v>2490</v>
       </c>
       <c r="Q253" s="3">
         <v>23039</v>
@@ -50778,12 +50733,7 @@
       <c r="AA253" s="1">
         <v>0</v>
       </c>
-      <c r="AC253" s="3">
-        <v>42309</v>
-      </c>
-      <c r="AD253" s="1" t="s">
-        <v>2401</v>
-      </c>
+      <c r="AC253" s="3"/>
       <c r="AF253" s="1" t="s">
         <v>103</v>
       </c>
@@ -50830,7 +50780,7 @@
         <v>108</v>
       </c>
       <c r="AZ253" s="1" t="s">
-        <v>2492</v>
+        <v>2491</v>
       </c>
       <c r="BB253" s="1">
         <v>1</v>
@@ -50845,10 +50795,10 @@
         <v>110</v>
       </c>
       <c r="BH253" s="1" t="s">
+        <v>2492</v>
+      </c>
+      <c r="BI253" s="1" t="s">
         <v>2493</v>
-      </c>
-      <c r="BI253" s="1" t="s">
-        <v>2494</v>
       </c>
       <c r="BM253" s="1" t="s">
         <v>113</v>
@@ -50860,13 +50810,13 @@
         <v>218</v>
       </c>
       <c r="BR253" s="1" t="s">
-        <v>2495</v>
+        <v>2494</v>
       </c>
       <c r="BS253" s="3">
         <v>34307</v>
       </c>
       <c r="BT253" s="1" t="s">
-        <v>2496</v>
+        <v>2495</v>
       </c>
       <c r="BU253" s="1" t="s">
         <v>117</v>
@@ -50884,13 +50834,13 @@
         <v>108</v>
       </c>
       <c r="CC253" s="1" t="s">
-        <v>2497</v>
+        <v>2496</v>
       </c>
       <c r="CD253" s="1" t="s">
         <v>456</v>
       </c>
       <c r="CE253" s="1" t="s">
-        <v>2498</v>
+        <v>2497</v>
       </c>
     </row>
     <row r="254" spans="1:83" x14ac:dyDescent="0.25">
@@ -50925,19 +50875,19 @@
         <v>93</v>
       </c>
       <c r="K254" s="1" t="s">
+        <v>2498</v>
+      </c>
+      <c r="L254" s="1" t="s">
         <v>2499</v>
       </c>
-      <c r="L254" s="1" t="s">
+      <c r="N254" s="1" t="s">
         <v>2500</v>
-      </c>
-      <c r="N254" s="1" t="s">
-        <v>2501</v>
       </c>
       <c r="O254" s="1" t="s">
         <v>97</v>
       </c>
       <c r="P254" s="1" t="s">
-        <v>2502</v>
+        <v>2501</v>
       </c>
       <c r="Q254" s="3">
         <v>23286</v>
@@ -50963,12 +50913,7 @@
       <c r="AA254" s="1">
         <v>0</v>
       </c>
-      <c r="AC254" s="3">
-        <v>42309</v>
-      </c>
-      <c r="AD254" s="1" t="s">
-        <v>2401</v>
-      </c>
+      <c r="AC254" s="3"/>
       <c r="AF254" s="1" t="s">
         <v>103</v>
       </c>
@@ -51018,7 +50963,7 @@
         <v>108</v>
       </c>
       <c r="AZ254" s="1" t="s">
-        <v>2503</v>
+        <v>2502</v>
       </c>
       <c r="BB254" s="1">
         <v>1</v>
@@ -51033,7 +50978,7 @@
         <v>110</v>
       </c>
       <c r="BH254" s="1" t="s">
-        <v>2504</v>
+        <v>2503</v>
       </c>
       <c r="BI254" s="1" t="s">
         <v>677</v>
@@ -51045,7 +50990,7 @@
         <v>102</v>
       </c>
       <c r="BT254" s="1" t="s">
-        <v>2505</v>
+        <v>2504</v>
       </c>
       <c r="BU254" s="1" t="s">
         <v>117</v>
@@ -51066,13 +51011,13 @@
         <v>108</v>
       </c>
       <c r="CC254" s="1" t="s">
+        <v>2505</v>
+      </c>
+      <c r="CD254" s="1" t="s">
         <v>2506</v>
       </c>
-      <c r="CD254" s="1" t="s">
+      <c r="CE254" s="1" t="s">
         <v>2507</v>
-      </c>
-      <c r="CE254" s="1" t="s">
-        <v>2508</v>
       </c>
     </row>
     <row r="255" spans="1:83" x14ac:dyDescent="0.25">
@@ -51107,19 +51052,19 @@
         <v>93</v>
       </c>
       <c r="K255" s="1" t="s">
+        <v>2508</v>
+      </c>
+      <c r="L255" s="1" t="s">
         <v>2509</v>
       </c>
-      <c r="L255" s="1" t="s">
+      <c r="N255" s="1" t="s">
         <v>2510</v>
-      </c>
-      <c r="N255" s="1" t="s">
-        <v>2511</v>
       </c>
       <c r="O255" s="1" t="s">
         <v>97</v>
       </c>
       <c r="P255" s="1" t="s">
-        <v>2512</v>
+        <v>2511</v>
       </c>
       <c r="Q255" s="3">
         <v>26907</v>
@@ -51142,12 +51087,7 @@
       <c r="AA255" s="1">
         <v>0</v>
       </c>
-      <c r="AC255" s="3">
-        <v>42309</v>
-      </c>
-      <c r="AD255" s="1" t="s">
-        <v>2401</v>
-      </c>
+      <c r="AC255" s="3"/>
       <c r="AF255" s="1" t="s">
         <v>103</v>
       </c>
@@ -51194,7 +51134,7 @@
         <v>108</v>
       </c>
       <c r="AZ255" s="1" t="s">
-        <v>2513</v>
+        <v>2512</v>
       </c>
       <c r="BB255" s="1">
         <v>1</v>
@@ -51209,10 +51149,10 @@
         <v>110</v>
       </c>
       <c r="BH255" s="1" t="s">
+        <v>2513</v>
+      </c>
+      <c r="BI255" s="1" t="s">
         <v>2514</v>
-      </c>
-      <c r="BI255" s="1" t="s">
-        <v>2515</v>
       </c>
       <c r="BM255" s="1" t="s">
         <v>113</v>
@@ -51224,13 +51164,13 @@
         <v>114</v>
       </c>
       <c r="BR255" s="1" t="s">
-        <v>2516</v>
+        <v>2515</v>
       </c>
       <c r="BS255" s="3">
         <v>35950</v>
       </c>
       <c r="BT255" s="1" t="s">
-        <v>2517</v>
+        <v>2516</v>
       </c>
       <c r="BU255" s="1" t="s">
         <v>117</v>
@@ -51248,13 +51188,13 @@
         <v>108</v>
       </c>
       <c r="CC255" s="1" t="s">
-        <v>2518</v>
+        <v>2517</v>
       </c>
       <c r="CD255" s="1" t="s">
         <v>1786</v>
       </c>
       <c r="CE255" s="1" t="s">
-        <v>2519</v>
+        <v>2518</v>
       </c>
     </row>
     <row r="256" spans="1:83" x14ac:dyDescent="0.25">
@@ -51289,19 +51229,19 @@
         <v>144</v>
       </c>
       <c r="K256" s="1" t="s">
+        <v>2519</v>
+      </c>
+      <c r="L256" s="1" t="s">
         <v>2520</v>
       </c>
-      <c r="L256" s="1" t="s">
+      <c r="N256" s="1" t="s">
         <v>2521</v>
-      </c>
-      <c r="N256" s="1" t="s">
-        <v>2522</v>
       </c>
       <c r="O256" s="1" t="s">
         <v>97</v>
       </c>
       <c r="P256" s="1" t="s">
-        <v>2523</v>
+        <v>2522</v>
       </c>
       <c r="Q256" s="3">
         <v>26349</v>
@@ -51346,7 +51286,7 @@
         <v>0</v>
       </c>
       <c r="AN256" s="1" t="s">
-        <v>2524</v>
+        <v>2523</v>
       </c>
       <c r="AO256" s="1">
         <v>0</v>
@@ -51385,13 +51325,13 @@
         <v>110</v>
       </c>
       <c r="BH256" s="1" t="s">
-        <v>2525</v>
+        <v>2524</v>
       </c>
       <c r="BM256" s="1" t="s">
         <v>113</v>
       </c>
       <c r="BT256" s="1" t="s">
-        <v>2526</v>
+        <v>2525</v>
       </c>
       <c r="BU256" s="1" t="s">
         <v>117</v>
@@ -51415,10 +51355,10 @@
         <v>2272</v>
       </c>
       <c r="CD256" s="1" t="s">
+        <v>2526</v>
+      </c>
+      <c r="CE256" s="1" t="s">
         <v>2527</v>
-      </c>
-      <c r="CE256" s="1" t="s">
-        <v>2528</v>
       </c>
     </row>
     <row r="257" spans="1:83" x14ac:dyDescent="0.25">
@@ -51453,19 +51393,19 @@
         <v>144</v>
       </c>
       <c r="K257" s="1" t="s">
+        <v>2528</v>
+      </c>
+      <c r="L257" s="1" t="s">
         <v>2529</v>
       </c>
-      <c r="L257" s="1" t="s">
+      <c r="N257" s="1" t="s">
         <v>2530</v>
-      </c>
-      <c r="N257" s="1" t="s">
-        <v>2531</v>
       </c>
       <c r="O257" s="1" t="s">
         <v>97</v>
       </c>
       <c r="P257" s="1" t="s">
-        <v>2532</v>
+        <v>2531</v>
       </c>
       <c r="Q257" s="3">
         <v>30589</v>
@@ -51513,7 +51453,7 @@
         <v>0</v>
       </c>
       <c r="AN257" s="1" t="s">
-        <v>2417</v>
+        <v>2416</v>
       </c>
       <c r="AO257" s="1">
         <v>0</v>
@@ -51552,13 +51492,13 @@
         <v>110</v>
       </c>
       <c r="BH257" s="1" t="s">
-        <v>2533</v>
+        <v>2532</v>
       </c>
       <c r="BM257" s="1" t="s">
         <v>113</v>
       </c>
       <c r="BT257" s="1" t="s">
-        <v>2534</v>
+        <v>2533</v>
       </c>
       <c r="BU257" s="1" t="s">
         <v>117</v>
@@ -51579,13 +51519,13 @@
         <v>108</v>
       </c>
       <c r="CC257" s="1" t="s">
+        <v>2534</v>
+      </c>
+      <c r="CD257" s="1" t="s">
         <v>2535</v>
       </c>
-      <c r="CD257" s="1" t="s">
+      <c r="CE257" s="1" t="s">
         <v>2536</v>
-      </c>
-      <c r="CE257" s="1" t="s">
-        <v>2537</v>
       </c>
     </row>
     <row r="258" spans="1:83" x14ac:dyDescent="0.25">
@@ -51620,19 +51560,19 @@
         <v>144</v>
       </c>
       <c r="K258" s="1" t="s">
+        <v>2537</v>
+      </c>
+      <c r="L258" s="1" t="s">
         <v>2538</v>
       </c>
-      <c r="L258" s="1" t="s">
+      <c r="N258" s="1" t="s">
         <v>2539</v>
-      </c>
-      <c r="N258" s="1" t="s">
-        <v>2540</v>
       </c>
       <c r="O258" s="1" t="s">
         <v>97</v>
       </c>
       <c r="P258" s="1" t="s">
-        <v>2541</v>
+        <v>2540</v>
       </c>
       <c r="Q258" s="3">
         <v>27354</v>
@@ -51680,7 +51620,7 @@
         <v>0</v>
       </c>
       <c r="AN258" s="1" t="s">
-        <v>2417</v>
+        <v>2416</v>
       </c>
       <c r="AO258" s="1">
         <v>0</v>
@@ -51719,13 +51659,13 @@
         <v>110</v>
       </c>
       <c r="BH258" s="1" t="s">
-        <v>2542</v>
+        <v>2541</v>
       </c>
       <c r="BM258" s="1" t="s">
         <v>113</v>
       </c>
       <c r="BT258" s="1" t="s">
-        <v>2543</v>
+        <v>2542</v>
       </c>
       <c r="BU258" s="1" t="s">
         <v>117</v>
@@ -51746,13 +51686,13 @@
         <v>108</v>
       </c>
       <c r="CC258" s="1" t="s">
+        <v>2543</v>
+      </c>
+      <c r="CD258" s="1" t="s">
         <v>2544</v>
       </c>
-      <c r="CD258" s="1" t="s">
+      <c r="CE258" s="1" t="s">
         <v>2545</v>
-      </c>
-      <c r="CE258" s="1" t="s">
-        <v>2546</v>
       </c>
     </row>
     <row r="259" spans="1:83" x14ac:dyDescent="0.25">
@@ -51787,19 +51727,19 @@
         <v>144</v>
       </c>
       <c r="K259" s="1" t="s">
+        <v>2546</v>
+      </c>
+      <c r="L259" s="1" t="s">
         <v>2547</v>
       </c>
-      <c r="L259" s="1" t="s">
+      <c r="N259" s="1" t="s">
         <v>2548</v>
-      </c>
-      <c r="N259" s="1" t="s">
-        <v>2549</v>
       </c>
       <c r="O259" s="1" t="s">
         <v>97</v>
       </c>
       <c r="P259" s="1" t="s">
-        <v>2550</v>
+        <v>2549</v>
       </c>
       <c r="Q259" s="3">
         <v>13756</v>
@@ -51883,13 +51823,13 @@
         <v>110</v>
       </c>
       <c r="BH259" s="1" t="s">
-        <v>2551</v>
+        <v>2550</v>
       </c>
       <c r="BM259" s="1" t="s">
         <v>113</v>
       </c>
       <c r="BT259" s="1" t="s">
-        <v>2552</v>
+        <v>2551</v>
       </c>
       <c r="BU259" s="1" t="s">
         <v>117</v>
@@ -51910,10 +51850,10 @@
         <v>108</v>
       </c>
       <c r="CC259" s="1" t="s">
-        <v>2405</v>
+        <v>2404</v>
       </c>
       <c r="CD259" s="1" t="s">
-        <v>2553</v>
+        <v>2552</v>
       </c>
       <c r="CE259" s="1" t="s">
         <v>209</v>
@@ -51951,19 +51891,19 @@
         <v>144</v>
       </c>
       <c r="K260" s="1" t="s">
+        <v>2553</v>
+      </c>
+      <c r="L260" s="1" t="s">
         <v>2554</v>
       </c>
-      <c r="L260" s="1" t="s">
+      <c r="N260" s="1" t="s">
         <v>2555</v>
-      </c>
-      <c r="N260" s="1" t="s">
-        <v>2556</v>
       </c>
       <c r="O260" s="1" t="s">
         <v>97</v>
       </c>
       <c r="P260" s="1" t="s">
-        <v>2557</v>
+        <v>2556</v>
       </c>
       <c r="Q260" s="3">
         <v>26074</v>
@@ -52011,7 +51951,7 @@
         <v>0</v>
       </c>
       <c r="AN260" s="1" t="s">
-        <v>2417</v>
+        <v>2416</v>
       </c>
       <c r="AO260" s="1">
         <v>0</v>
@@ -52050,13 +51990,13 @@
         <v>110</v>
       </c>
       <c r="BH260" s="1" t="s">
-        <v>2533</v>
+        <v>2532</v>
       </c>
       <c r="BM260" s="1" t="s">
         <v>113</v>
       </c>
       <c r="BT260" s="1" t="s">
-        <v>2558</v>
+        <v>2557</v>
       </c>
       <c r="BU260" s="1" t="s">
         <v>117</v>
@@ -52080,13 +52020,13 @@
         <v>108</v>
       </c>
       <c r="CC260" s="1" t="s">
-        <v>2559</v>
+        <v>2558</v>
       </c>
       <c r="CD260" s="1" t="s">
         <v>1255</v>
       </c>
       <c r="CE260" s="1" t="s">
-        <v>2560</v>
+        <v>2559</v>
       </c>
     </row>
     <row r="261" spans="1:83" x14ac:dyDescent="0.25">
@@ -52121,19 +52061,19 @@
         <v>144</v>
       </c>
       <c r="K261" s="1" t="s">
+        <v>2560</v>
+      </c>
+      <c r="L261" s="1" t="s">
         <v>2561</v>
       </c>
-      <c r="L261" s="1" t="s">
+      <c r="N261" s="1" t="s">
         <v>2562</v>
-      </c>
-      <c r="N261" s="1" t="s">
-        <v>2563</v>
       </c>
       <c r="O261" s="1" t="s">
         <v>97</v>
       </c>
       <c r="P261" s="1" t="s">
-        <v>2564</v>
+        <v>2563</v>
       </c>
       <c r="Q261" s="3">
         <v>28808</v>
@@ -52178,7 +52118,7 @@
         <v>0</v>
       </c>
       <c r="AN261" s="1" t="s">
-        <v>2565</v>
+        <v>2564</v>
       </c>
       <c r="AO261" s="1">
         <v>0</v>
@@ -52217,13 +52157,13 @@
         <v>110</v>
       </c>
       <c r="BH261" s="1" t="s">
-        <v>2566</v>
+        <v>2565</v>
       </c>
       <c r="BM261" s="1" t="s">
         <v>113</v>
       </c>
       <c r="BT261" s="1" t="s">
-        <v>2567</v>
+        <v>2566</v>
       </c>
       <c r="BU261" s="1" t="s">
         <v>117</v>
@@ -52244,18 +52184,18 @@
         <v>108</v>
       </c>
       <c r="CC261" s="1" t="s">
+        <v>2567</v>
+      </c>
+      <c r="CD261" s="1" t="s">
+        <v>2474</v>
+      </c>
+      <c r="CE261" s="1" t="s">
         <v>2568</v>
-      </c>
-      <c r="CD261" s="1" t="s">
-        <v>2475</v>
-      </c>
-      <c r="CE261" s="1" t="s">
-        <v>2569</v>
       </c>
     </row>
     <row r="262" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
-        <v>2570</v>
+        <v>2569</v>
       </c>
       <c r="B262" s="1" t="s">
         <v>85</v>
@@ -52267,7 +52207,7 @@
         <v>124</v>
       </c>
       <c r="E262" s="1" t="s">
-        <v>2571</v>
+        <v>2570</v>
       </c>
       <c r="F262" s="1" t="s">
         <v>108</v>
@@ -52279,22 +52219,22 @@
         <v>91</v>
       </c>
       <c r="I262" s="1" t="s">
-        <v>2572</v>
+        <v>2571</v>
       </c>
       <c r="J262" s="1" t="s">
         <v>93</v>
       </c>
       <c r="K262" s="1" t="s">
+        <v>2572</v>
+      </c>
+      <c r="L262" s="1" t="s">
         <v>2573</v>
       </c>
-      <c r="L262" s="1" t="s">
+      <c r="M262" s="1" t="s">
         <v>2574</v>
       </c>
-      <c r="M262" s="1" t="s">
+      <c r="N262" s="1" t="s">
         <v>2575</v>
-      </c>
-      <c r="N262" s="1" t="s">
-        <v>2576</v>
       </c>
       <c r="Q262" s="3">
         <v>21430</v>
@@ -52327,7 +52267,7 @@
         <v>41330</v>
       </c>
       <c r="AD262" s="1" t="s">
-        <v>2577</v>
+        <v>2576</v>
       </c>
       <c r="AF262" s="1" t="s">
         <v>103</v>
@@ -52378,10 +52318,10 @@
         <v>108</v>
       </c>
       <c r="BH262" s="1" t="s">
+        <v>2577</v>
+      </c>
+      <c r="BI262" s="1" t="s">
         <v>2578</v>
-      </c>
-      <c r="BI262" s="1" t="s">
-        <v>2579</v>
       </c>
       <c r="BM262" s="1" t="s">
         <v>113</v>
@@ -52390,7 +52330,7 @@
         <v>102</v>
       </c>
       <c r="BT262" s="1" t="s">
-        <v>2580</v>
+        <v>2579</v>
       </c>
       <c r="BU262" s="1" t="s">
         <v>117</v>
@@ -52414,13 +52354,13 @@
         <v>108</v>
       </c>
       <c r="CC262" s="1" t="s">
+        <v>2580</v>
+      </c>
+      <c r="CD262" s="1" t="s">
         <v>2581</v>
       </c>
-      <c r="CD262" s="1" t="s">
+      <c r="CE262" s="1" t="s">
         <v>2582</v>
-      </c>
-      <c r="CE262" s="1" t="s">
-        <v>2583</v>
       </c>
     </row>
     <row r="263" spans="1:83" x14ac:dyDescent="0.25">
@@ -52455,16 +52395,16 @@
         <v>93</v>
       </c>
       <c r="K263" s="1" t="s">
+        <v>2583</v>
+      </c>
+      <c r="L263" s="1" t="s">
         <v>2584</v>
       </c>
-      <c r="L263" s="1" t="s">
+      <c r="M263" s="1" t="s">
+        <v>2574</v>
+      </c>
+      <c r="N263" s="1" t="s">
         <v>2585</v>
-      </c>
-      <c r="M263" s="1" t="s">
-        <v>2575</v>
-      </c>
-      <c r="N263" s="1" t="s">
-        <v>2586</v>
       </c>
       <c r="Q263" s="3">
         <v>21965</v>
@@ -52491,13 +52431,13 @@
         <v>0</v>
       </c>
       <c r="AB263" s="1" t="s">
-        <v>2587</v>
+        <v>2586</v>
       </c>
       <c r="AC263" s="3">
         <v>41579</v>
       </c>
       <c r="AD263" s="1" t="s">
-        <v>2588</v>
+        <v>2587</v>
       </c>
       <c r="AF263" s="1" t="s">
         <v>103</v>
@@ -52545,13 +52485,13 @@
         <v>108</v>
       </c>
       <c r="AZ263" s="1" t="s">
-        <v>2589</v>
+        <v>2588</v>
       </c>
       <c r="BD263" s="1" t="s">
         <v>99</v>
       </c>
       <c r="BH263" s="1" t="s">
-        <v>2590</v>
+        <v>2589</v>
       </c>
       <c r="BM263" s="1" t="s">
         <v>113</v>
@@ -52563,13 +52503,13 @@
         <v>218</v>
       </c>
       <c r="BR263" s="1" t="s">
-        <v>2591</v>
+        <v>2590</v>
       </c>
       <c r="BS263" s="3">
         <v>35087</v>
       </c>
       <c r="BT263" s="1" t="s">
-        <v>2592</v>
+        <v>2591</v>
       </c>
       <c r="BU263" s="1" t="s">
         <v>117</v>
@@ -52590,13 +52530,13 @@
         <v>108</v>
       </c>
       <c r="CC263" s="1" t="s">
-        <v>2593</v>
+        <v>2592</v>
       </c>
       <c r="CD263" s="1" t="s">
         <v>1628</v>
       </c>
       <c r="CE263" s="1" t="s">
-        <v>2594</v>
+        <v>2593</v>
       </c>
     </row>
     <row r="264" spans="1:83" x14ac:dyDescent="0.25">
@@ -52613,7 +52553,7 @@
         <v>124</v>
       </c>
       <c r="E264" s="1" t="s">
-        <v>2595</v>
+        <v>2594</v>
       </c>
       <c r="F264" s="1" t="s">
         <v>108</v>
@@ -52625,22 +52565,22 @@
         <v>91</v>
       </c>
       <c r="I264" s="1" t="s">
-        <v>2596</v>
+        <v>2595</v>
       </c>
       <c r="J264" s="1" t="s">
         <v>93</v>
       </c>
       <c r="K264" s="1" t="s">
+        <v>2596</v>
+      </c>
+      <c r="L264" s="1" t="s">
         <v>2597</v>
       </c>
-      <c r="L264" s="1" t="s">
+      <c r="M264" s="1" t="s">
+        <v>2574</v>
+      </c>
+      <c r="N264" s="1" t="s">
         <v>2598</v>
-      </c>
-      <c r="M264" s="1" t="s">
-        <v>2575</v>
-      </c>
-      <c r="N264" s="1" t="s">
-        <v>2599</v>
       </c>
       <c r="Q264" s="3">
         <v>18241</v>
@@ -52667,7 +52607,7 @@
         <v>41759</v>
       </c>
       <c r="AD264" s="1" t="s">
-        <v>2600</v>
+        <v>2599</v>
       </c>
       <c r="AF264" s="1" t="s">
         <v>103</v>
@@ -52697,28 +52637,28 @@
         <v>107</v>
       </c>
       <c r="AQ264" s="1" t="s">
+        <v>2600</v>
+      </c>
+      <c r="AR264" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS264" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT264" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU264" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV264" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY264" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="BH264" s="1" t="s">
         <v>2601</v>
-      </c>
-      <c r="AR264" s="1">
-        <v>0</v>
-      </c>
-      <c r="AS264" s="1">
-        <v>0</v>
-      </c>
-      <c r="AT264" s="1">
-        <v>0</v>
-      </c>
-      <c r="AU264" s="1">
-        <v>0</v>
-      </c>
-      <c r="AV264" s="1">
-        <v>0</v>
-      </c>
-      <c r="AY264" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="BH264" s="1" t="s">
-        <v>2602</v>
       </c>
       <c r="BM264" s="1" t="s">
         <v>113</v>
@@ -52727,13 +52667,13 @@
         <v>114</v>
       </c>
       <c r="BR264" s="1" t="s">
-        <v>2603</v>
+        <v>2602</v>
       </c>
       <c r="BS264" s="3">
         <v>34292</v>
       </c>
       <c r="BT264" s="1" t="s">
-        <v>2604</v>
+        <v>2603</v>
       </c>
       <c r="BU264" s="1" t="s">
         <v>117</v>
@@ -52754,7 +52694,7 @@
         <v>108</v>
       </c>
       <c r="CC264" s="1" t="s">
-        <v>2605</v>
+        <v>2604</v>
       </c>
       <c r="CD264" s="1" t="s">
         <v>1837</v>
@@ -52795,19 +52735,19 @@
         <v>93</v>
       </c>
       <c r="K265" s="1" t="s">
+        <v>2605</v>
+      </c>
+      <c r="L265" s="1" t="s">
         <v>2606</v>
       </c>
-      <c r="L265" s="1" t="s">
+      <c r="N265" s="1" t="s">
         <v>2607</v>
-      </c>
-      <c r="N265" s="1" t="s">
-        <v>2608</v>
       </c>
       <c r="O265" s="1" t="s">
         <v>97</v>
       </c>
       <c r="P265" s="1" t="s">
-        <v>2609</v>
+        <v>2608</v>
       </c>
       <c r="Q265" s="3">
         <v>23125</v>
@@ -52840,7 +52780,7 @@
         <v>42247</v>
       </c>
       <c r="AD265" s="1" t="s">
-        <v>2610</v>
+        <v>2609</v>
       </c>
       <c r="AF265" s="1" t="s">
         <v>103</v>
@@ -52900,10 +52840,10 @@
         <v>110</v>
       </c>
       <c r="BH265" s="1" t="s">
+        <v>2610</v>
+      </c>
+      <c r="BI265" s="1" t="s">
         <v>2611</v>
-      </c>
-      <c r="BI265" s="1" t="s">
-        <v>2612</v>
       </c>
       <c r="BM265" s="1" t="s">
         <v>113</v>
@@ -52915,13 +52855,13 @@
         <v>218</v>
       </c>
       <c r="BR265" s="1" t="s">
-        <v>2613</v>
+        <v>2612</v>
       </c>
       <c r="BS265" s="3">
         <v>36580</v>
       </c>
       <c r="BT265" s="1" t="s">
-        <v>2614</v>
+        <v>2613</v>
       </c>
       <c r="BU265" s="1" t="s">
         <v>117</v>
@@ -52942,7 +52882,7 @@
         <v>108</v>
       </c>
       <c r="CC265" s="1" t="s">
-        <v>2615</v>
+        <v>2614</v>
       </c>
       <c r="CD265" s="1" t="s">
         <v>318</v>
@@ -52983,16 +52923,16 @@
         <v>93</v>
       </c>
       <c r="K266" s="1" t="s">
+        <v>2615</v>
+      </c>
+      <c r="L266" s="1" t="s">
         <v>2616</v>
       </c>
-      <c r="L266" s="1" t="s">
+      <c r="M266" s="1" t="s">
+        <v>2574</v>
+      </c>
+      <c r="N266" s="1" t="s">
         <v>2617</v>
-      </c>
-      <c r="M266" s="1" t="s">
-        <v>2575</v>
-      </c>
-      <c r="N266" s="1" t="s">
-        <v>2618</v>
       </c>
       <c r="Q266" s="3">
         <v>23356</v>
@@ -53015,12 +52955,7 @@
       <c r="AA266" s="1">
         <v>0</v>
       </c>
-      <c r="AC266" s="3">
-        <v>42308</v>
-      </c>
-      <c r="AD266" s="1" t="s">
-        <v>2401</v>
-      </c>
+      <c r="AC266" s="3"/>
       <c r="AF266" s="1" t="s">
         <v>103</v>
       </c>
@@ -53067,7 +53002,7 @@
         <v>108</v>
       </c>
       <c r="BH266" s="1" t="s">
-        <v>2619</v>
+        <v>2618</v>
       </c>
       <c r="BM266" s="1" t="s">
         <v>113</v>
@@ -53079,13 +53014,13 @@
         <v>99</v>
       </c>
       <c r="BR266" s="1" t="s">
-        <v>2620</v>
+        <v>2619</v>
       </c>
       <c r="BS266" s="3">
         <v>34412</v>
       </c>
       <c r="BT266" s="1" t="s">
-        <v>2621</v>
+        <v>2620</v>
       </c>
       <c r="BU266" s="1" t="s">
         <v>117</v>
@@ -53106,13 +53041,13 @@
         <v>108</v>
       </c>
       <c r="CC266" s="1" t="s">
+        <v>2621</v>
+      </c>
+      <c r="CD266" s="1" t="s">
         <v>2622</v>
       </c>
-      <c r="CD266" s="1" t="s">
+      <c r="CE266" s="1" t="s">
         <v>2623</v>
-      </c>
-      <c r="CE266" s="1" t="s">
-        <v>2624</v>
       </c>
     </row>
     <row r="267" spans="1:83" x14ac:dyDescent="0.25">
@@ -53150,10 +53085,10 @@
         <v>2243</v>
       </c>
       <c r="L267" s="1" t="s">
-        <v>2625</v>
+        <v>2624</v>
       </c>
       <c r="M267" s="1" t="s">
-        <v>2575</v>
+        <v>2574</v>
       </c>
       <c r="N267" s="1" t="s">
         <v>2245</v>
@@ -53179,12 +53114,7 @@
       <c r="AA267" s="1">
         <v>0</v>
       </c>
-      <c r="AC267" s="3">
-        <v>42369</v>
-      </c>
-      <c r="AD267" s="1" t="s">
-        <v>2401</v>
-      </c>
+      <c r="AC267" s="3"/>
       <c r="AF267" s="1" t="s">
         <v>103</v>
       </c>
@@ -53234,10 +53164,10 @@
         <v>108</v>
       </c>
       <c r="BH267" s="1" t="s">
+        <v>2625</v>
+      </c>
+      <c r="BI267" s="1" t="s">
         <v>2626</v>
-      </c>
-      <c r="BI267" s="1" t="s">
-        <v>2627</v>
       </c>
       <c r="BM267" s="1" t="s">
         <v>113</v>
@@ -53302,19 +53232,19 @@
         <v>93</v>
       </c>
       <c r="K268" s="1" t="s">
+        <v>2627</v>
+      </c>
+      <c r="L268" s="1" t="s">
         <v>2628</v>
       </c>
-      <c r="L268" s="1" t="s">
+      <c r="N268" s="1" t="s">
         <v>2629</v>
-      </c>
-      <c r="N268" s="1" t="s">
-        <v>2630</v>
       </c>
       <c r="O268" s="1" t="s">
         <v>97</v>
       </c>
       <c r="P268" s="1" t="s">
-        <v>2631</v>
+        <v>2630</v>
       </c>
       <c r="Q268" s="3">
         <v>24907</v>
@@ -53395,13 +53325,13 @@
         <v>110</v>
       </c>
       <c r="BH268" s="1" t="s">
+        <v>2631</v>
+      </c>
+      <c r="BI268" s="1" t="s">
         <v>2632</v>
       </c>
-      <c r="BI268" s="1" t="s">
+      <c r="BJ268" s="1" t="s">
         <v>2633</v>
-      </c>
-      <c r="BJ268" s="1" t="s">
-        <v>2634</v>
       </c>
       <c r="BM268" s="1" t="s">
         <v>113</v>
@@ -53416,7 +53346,7 @@
         <v>35679</v>
       </c>
       <c r="BT268" s="1" t="s">
-        <v>2635</v>
+        <v>2634</v>
       </c>
       <c r="BU268" s="1" t="s">
         <v>117</v>
@@ -53434,7 +53364,7 @@
         <v>89</v>
       </c>
       <c r="CC268" s="1" t="s">
-        <v>2636</v>
+        <v>2635</v>
       </c>
       <c r="CD268" s="1" t="s">
         <v>283</v>
@@ -53475,19 +53405,19 @@
         <v>93</v>
       </c>
       <c r="K269" s="1" t="s">
+        <v>2636</v>
+      </c>
+      <c r="L269" s="1" t="s">
         <v>2637</v>
       </c>
-      <c r="L269" s="1" t="s">
+      <c r="N269" s="1" t="s">
         <v>2638</v>
-      </c>
-      <c r="N269" s="1" t="s">
-        <v>2639</v>
       </c>
       <c r="O269" s="1" t="s">
         <v>97</v>
       </c>
       <c r="P269" s="1" t="s">
-        <v>2640</v>
+        <v>2639</v>
       </c>
       <c r="Q269" s="3">
         <v>28642</v>
@@ -53562,7 +53492,7 @@
         <v>108</v>
       </c>
       <c r="AZ269" s="1" t="s">
-        <v>2641</v>
+        <v>2640</v>
       </c>
       <c r="BB269" s="1">
         <v>1</v>
@@ -53574,7 +53504,7 @@
         <v>110</v>
       </c>
       <c r="BH269" s="1" t="s">
-        <v>2642</v>
+        <v>2641</v>
       </c>
       <c r="BM269" s="1" t="s">
         <v>113</v>
@@ -53583,7 +53513,7 @@
         <v>102</v>
       </c>
       <c r="BT269" s="1" t="s">
-        <v>2643</v>
+        <v>2642</v>
       </c>
       <c r="BU269" s="1" t="s">
         <v>117</v>
@@ -53601,13 +53531,13 @@
         <v>108</v>
       </c>
       <c r="CC269" s="1" t="s">
-        <v>2644</v>
+        <v>2643</v>
       </c>
       <c r="CD269" s="1" t="s">
         <v>456</v>
       </c>
       <c r="CE269" s="1" t="s">
-        <v>2645</v>
+        <v>2644</v>
       </c>
     </row>
     <row r="270" spans="1:83" x14ac:dyDescent="0.25">
@@ -53642,19 +53572,19 @@
         <v>93</v>
       </c>
       <c r="K270" s="1" t="s">
+        <v>2645</v>
+      </c>
+      <c r="L270" s="1" t="s">
         <v>2646</v>
       </c>
-      <c r="L270" s="1" t="s">
+      <c r="N270" s="1" t="s">
         <v>2647</v>
-      </c>
-      <c r="N270" s="1" t="s">
-        <v>2648</v>
       </c>
       <c r="O270" s="1" t="s">
         <v>97</v>
       </c>
       <c r="P270" s="1" t="s">
-        <v>2649</v>
+        <v>2648</v>
       </c>
       <c r="Q270" s="3">
         <v>28239</v>
@@ -53726,7 +53656,7 @@
         <v>108</v>
       </c>
       <c r="AZ270" s="1" t="s">
-        <v>2650</v>
+        <v>2649</v>
       </c>
       <c r="BB270" s="1">
         <v>1</v>
@@ -53738,7 +53668,7 @@
         <v>110</v>
       </c>
       <c r="BH270" s="1" t="s">
-        <v>2651</v>
+        <v>2650</v>
       </c>
       <c r="BM270" s="1" t="s">
         <v>113</v>
@@ -53750,13 +53680,13 @@
         <v>218</v>
       </c>
       <c r="BR270" s="1" t="s">
-        <v>2652</v>
+        <v>2651</v>
       </c>
       <c r="BS270" s="3">
         <v>36099</v>
       </c>
       <c r="BT270" s="1" t="s">
-        <v>2653</v>
+        <v>2652</v>
       </c>
       <c r="BU270" s="1" t="s">
         <v>117</v>
@@ -53774,13 +53704,13 @@
         <v>108</v>
       </c>
       <c r="CC270" s="1" t="s">
+        <v>2653</v>
+      </c>
+      <c r="CD270" s="1" t="s">
         <v>2654</v>
       </c>
-      <c r="CD270" s="1" t="s">
+      <c r="CE270" s="1" t="s">
         <v>2655</v>
-      </c>
-      <c r="CE270" s="1" t="s">
-        <v>2656</v>
       </c>
     </row>
     <row r="271" spans="1:83" x14ac:dyDescent="0.25">
@@ -53815,19 +53745,19 @@
         <v>93</v>
       </c>
       <c r="K271" s="1" t="s">
+        <v>2656</v>
+      </c>
+      <c r="L271" s="1" t="s">
         <v>2657</v>
       </c>
-      <c r="L271" s="1" t="s">
+      <c r="N271" s="1" t="s">
         <v>2658</v>
-      </c>
-      <c r="N271" s="1" t="s">
-        <v>2659</v>
       </c>
       <c r="O271" s="1" t="s">
         <v>97</v>
       </c>
       <c r="P271" s="1" t="s">
-        <v>2660</v>
+        <v>2659</v>
       </c>
       <c r="Q271" s="3">
         <v>25589</v>
@@ -53899,7 +53829,7 @@
         <v>108</v>
       </c>
       <c r="AZ271" s="1" t="s">
-        <v>2661</v>
+        <v>2660</v>
       </c>
       <c r="BB271" s="1">
         <v>1</v>
@@ -53911,7 +53841,7 @@
         <v>110</v>
       </c>
       <c r="BH271" s="1" t="s">
-        <v>2662</v>
+        <v>2661</v>
       </c>
       <c r="BM271" s="1" t="s">
         <v>113</v>
@@ -53923,13 +53853,13 @@
         <v>99</v>
       </c>
       <c r="BR271" s="1" t="s">
-        <v>2663</v>
+        <v>2662</v>
       </c>
       <c r="BS271" s="3">
         <v>37735</v>
       </c>
       <c r="BT271" s="1" t="s">
-        <v>2664</v>
+        <v>2663</v>
       </c>
       <c r="BU271" s="1" t="s">
         <v>117</v>
@@ -53947,13 +53877,13 @@
         <v>108</v>
       </c>
       <c r="CC271" s="1" t="s">
+        <v>2664</v>
+      </c>
+      <c r="CD271" s="1" t="s">
         <v>2665</v>
       </c>
-      <c r="CD271" s="1" t="s">
+      <c r="CE271" s="1" t="s">
         <v>2666</v>
-      </c>
-      <c r="CE271" s="1" t="s">
-        <v>2667</v>
       </c>
     </row>
     <row r="272" spans="1:83" x14ac:dyDescent="0.25">
@@ -53988,19 +53918,19 @@
         <v>93</v>
       </c>
       <c r="K272" s="1" t="s">
+        <v>2667</v>
+      </c>
+      <c r="L272" s="1" t="s">
         <v>2668</v>
       </c>
-      <c r="L272" s="1" t="s">
+      <c r="N272" s="1" t="s">
         <v>2669</v>
-      </c>
-      <c r="N272" s="1" t="s">
-        <v>2670</v>
       </c>
       <c r="O272" s="1" t="s">
         <v>97</v>
       </c>
       <c r="P272" s="1" t="s">
-        <v>2671</v>
+        <v>2670</v>
       </c>
       <c r="Q272" s="3">
         <v>29170</v>
@@ -54075,7 +54005,7 @@
         <v>108</v>
       </c>
       <c r="AZ272" s="1" t="s">
-        <v>2672</v>
+        <v>2671</v>
       </c>
       <c r="BB272" s="1">
         <v>1</v>
@@ -54087,7 +54017,7 @@
         <v>110</v>
       </c>
       <c r="BH272" s="1" t="s">
-        <v>2673</v>
+        <v>2672</v>
       </c>
       <c r="BM272" s="1" t="s">
         <v>113</v>
@@ -54096,7 +54026,7 @@
         <v>102</v>
       </c>
       <c r="BT272" s="1" t="s">
-        <v>2674</v>
+        <v>2673</v>
       </c>
       <c r="BU272" s="1" t="s">
         <v>117</v>
@@ -54114,13 +54044,13 @@
         <v>108</v>
       </c>
       <c r="CC272" s="1" t="s">
-        <v>2675</v>
+        <v>2674</v>
       </c>
       <c r="CD272" s="1" t="s">
         <v>890</v>
       </c>
       <c r="CE272" s="1" t="s">
-        <v>2676</v>
+        <v>2675</v>
       </c>
     </row>
     <row r="273" spans="1:83" x14ac:dyDescent="0.25">
@@ -54155,19 +54085,19 @@
         <v>93</v>
       </c>
       <c r="K273" s="1" t="s">
+        <v>2676</v>
+      </c>
+      <c r="L273" s="1" t="s">
         <v>2677</v>
       </c>
-      <c r="L273" s="1" t="s">
+      <c r="N273" s="1" t="s">
         <v>2678</v>
-      </c>
-      <c r="N273" s="1" t="s">
-        <v>2679</v>
       </c>
       <c r="O273" s="1" t="s">
         <v>97</v>
       </c>
       <c r="P273" s="1" t="s">
-        <v>2680</v>
+        <v>2679</v>
       </c>
       <c r="Q273" s="3">
         <v>27250</v>
@@ -54197,7 +54127,7 @@
         <v>103</v>
       </c>
       <c r="AG273" s="1" t="s">
-        <v>2681</v>
+        <v>2680</v>
       </c>
       <c r="AH273" s="1" t="s">
         <v>1893</v>
@@ -54242,7 +54172,7 @@
         <v>108</v>
       </c>
       <c r="AZ273" s="1" t="s">
-        <v>2682</v>
+        <v>2681</v>
       </c>
       <c r="BB273" s="1">
         <v>1</v>
@@ -54254,7 +54184,7 @@
         <v>110</v>
       </c>
       <c r="BH273" s="1" t="s">
-        <v>2683</v>
+        <v>2682</v>
       </c>
       <c r="BM273" s="1" t="s">
         <v>113</v>
@@ -54263,7 +54193,7 @@
         <v>102</v>
       </c>
       <c r="BT273" s="1" t="s">
-        <v>2684</v>
+        <v>2683</v>
       </c>
       <c r="BU273" s="1" t="s">
         <v>117</v>
@@ -54284,10 +54214,10 @@
         <v>1576</v>
       </c>
       <c r="CD273" s="1" t="s">
+        <v>2684</v>
+      </c>
+      <c r="CE273" s="1" t="s">
         <v>2685</v>
-      </c>
-      <c r="CE273" s="1" t="s">
-        <v>2686</v>
       </c>
     </row>
     <row r="274" spans="1:83" x14ac:dyDescent="0.25">
@@ -54322,19 +54252,19 @@
         <v>93</v>
       </c>
       <c r="K274" s="1" t="s">
+        <v>2686</v>
+      </c>
+      <c r="L274" s="1" t="s">
         <v>2687</v>
       </c>
-      <c r="L274" s="1" t="s">
+      <c r="N274" s="1" t="s">
         <v>2688</v>
-      </c>
-      <c r="N274" s="1" t="s">
-        <v>2689</v>
       </c>
       <c r="O274" s="1" t="s">
         <v>97</v>
       </c>
       <c r="P274" s="1" t="s">
-        <v>2690</v>
+        <v>2689</v>
       </c>
       <c r="Q274" s="3">
         <v>27999</v>
@@ -54409,7 +54339,7 @@
         <v>108</v>
       </c>
       <c r="AZ274" s="1" t="s">
-        <v>2691</v>
+        <v>2690</v>
       </c>
       <c r="BB274" s="1">
         <v>1</v>
@@ -54430,7 +54360,7 @@
         <v>102</v>
       </c>
       <c r="BT274" s="1" t="s">
-        <v>2692</v>
+        <v>2691</v>
       </c>
       <c r="BU274" s="1" t="s">
         <v>117</v>
@@ -54454,7 +54384,7 @@
         <v>973</v>
       </c>
       <c r="CE274" s="1" t="s">
-        <v>2693</v>
+        <v>2692</v>
       </c>
     </row>
     <row r="275" spans="1:83" x14ac:dyDescent="0.25">
@@ -54489,19 +54419,19 @@
         <v>93</v>
       </c>
       <c r="K275" s="1" t="s">
+        <v>2693</v>
+      </c>
+      <c r="L275" s="1" t="s">
         <v>2694</v>
       </c>
-      <c r="L275" s="1" t="s">
+      <c r="N275" s="1" t="s">
         <v>2695</v>
-      </c>
-      <c r="N275" s="1" t="s">
-        <v>2696</v>
       </c>
       <c r="O275" s="1" t="s">
         <v>97</v>
       </c>
       <c r="P275" s="1" t="s">
-        <v>2697</v>
+        <v>2696</v>
       </c>
       <c r="Q275" s="3">
         <v>29305</v>
@@ -54534,7 +54464,7 @@
         <v>686</v>
       </c>
       <c r="AH275" s="1" t="s">
-        <v>2698</v>
+        <v>2697</v>
       </c>
       <c r="AI275" s="1" t="s">
         <v>108</v>
@@ -54576,7 +54506,7 @@
         <v>108</v>
       </c>
       <c r="AZ275" s="1" t="s">
-        <v>2699</v>
+        <v>2698</v>
       </c>
       <c r="BB275" s="1">
         <v>1</v>
@@ -54588,7 +54518,7 @@
         <v>110</v>
       </c>
       <c r="BH275" s="1" t="s">
-        <v>2700</v>
+        <v>2699</v>
       </c>
       <c r="BM275" s="1" t="s">
         <v>113</v>
@@ -54597,7 +54527,7 @@
         <v>102</v>
       </c>
       <c r="BT275" s="1" t="s">
-        <v>2701</v>
+        <v>2700</v>
       </c>
       <c r="BU275" s="1" t="s">
         <v>117</v>
@@ -54615,13 +54545,13 @@
         <v>108</v>
       </c>
       <c r="CC275" s="1" t="s">
+        <v>2701</v>
+      </c>
+      <c r="CD275" s="1" t="s">
         <v>2702</v>
       </c>
-      <c r="CD275" s="1" t="s">
+      <c r="CE275" s="1" t="s">
         <v>2703</v>
-      </c>
-      <c r="CE275" s="1" t="s">
-        <v>2704</v>
       </c>
     </row>
     <row r="276" spans="1:83" x14ac:dyDescent="0.25">
@@ -54656,19 +54586,19 @@
         <v>144</v>
       </c>
       <c r="K276" s="1" t="s">
+        <v>2704</v>
+      </c>
+      <c r="L276" s="1" t="s">
         <v>2705</v>
       </c>
-      <c r="L276" s="1" t="s">
+      <c r="N276" s="1" t="s">
         <v>2706</v>
-      </c>
-      <c r="N276" s="1" t="s">
-        <v>2707</v>
       </c>
       <c r="O276" s="1" t="s">
         <v>97</v>
       </c>
       <c r="P276" s="1" t="s">
-        <v>2708</v>
+        <v>2707</v>
       </c>
       <c r="R276" s="1" t="s">
         <v>131</v>
@@ -54704,7 +54634,7 @@
         <v>0</v>
       </c>
       <c r="AN276" s="1" t="s">
-        <v>2709</v>
+        <v>2708</v>
       </c>
       <c r="AO276" s="1">
         <v>0</v>
@@ -54737,13 +54667,13 @@
         <v>110</v>
       </c>
       <c r="BH276" s="1" t="s">
-        <v>2710</v>
+        <v>2709</v>
       </c>
       <c r="BM276" s="1" t="s">
         <v>113</v>
       </c>
       <c r="BT276" s="1" t="s">
-        <v>2711</v>
+        <v>2710</v>
       </c>
       <c r="BU276" s="1" t="s">
         <v>117</v>
@@ -54761,13 +54691,13 @@
         <v>108</v>
       </c>
       <c r="CC276" s="1" t="s">
-        <v>2712</v>
+        <v>2711</v>
       </c>
       <c r="CD276" s="1" t="s">
         <v>329</v>
       </c>
       <c r="CE276" s="1" t="s">
-        <v>2713</v>
+        <v>2712</v>
       </c>
     </row>
     <row r="277" spans="1:83" x14ac:dyDescent="0.25">
@@ -54802,16 +54732,16 @@
         <v>93</v>
       </c>
       <c r="K277" s="1" t="s">
+        <v>2713</v>
+      </c>
+      <c r="L277" s="1" t="s">
         <v>2714</v>
       </c>
-      <c r="L277" s="1" t="s">
+      <c r="M277" s="1" t="s">
+        <v>2574</v>
+      </c>
+      <c r="N277" s="1" t="s">
         <v>2715</v>
-      </c>
-      <c r="M277" s="1" t="s">
-        <v>2575</v>
-      </c>
-      <c r="N277" s="1" t="s">
-        <v>2716</v>
       </c>
       <c r="Q277" s="3">
         <v>18523</v>
@@ -54844,7 +54774,7 @@
         <v>42379</v>
       </c>
       <c r="AD277" s="1" t="s">
-        <v>2717</v>
+        <v>2716</v>
       </c>
       <c r="AF277" s="1" t="s">
         <v>250</v>
@@ -54874,37 +54804,37 @@
         <v>251</v>
       </c>
       <c r="AQ277" s="1" t="s">
+        <v>2717</v>
+      </c>
+      <c r="AR277" s="1">
+        <v>0</v>
+      </c>
+      <c r="AS277" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT277" s="1">
+        <v>0</v>
+      </c>
+      <c r="AU277" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV277" s="1">
+        <v>0</v>
+      </c>
+      <c r="AY277" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="AZ277" s="1" t="s">
         <v>2718</v>
-      </c>
-      <c r="AR277" s="1">
-        <v>0</v>
-      </c>
-      <c r="AS277" s="1">
-        <v>0</v>
-      </c>
-      <c r="AT277" s="1">
-        <v>0</v>
-      </c>
-      <c r="AU277" s="1">
-        <v>0</v>
-      </c>
-      <c r="AV277" s="1">
-        <v>0</v>
-      </c>
-      <c r="AY277" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="AZ277" s="1" t="s">
-        <v>2719</v>
       </c>
       <c r="BD277" s="1" t="s">
         <v>433</v>
       </c>
       <c r="BH277" s="1" t="s">
+        <v>2719</v>
+      </c>
+      <c r="BI277" s="1" t="s">
         <v>2720</v>
-      </c>
-      <c r="BI277" s="1" t="s">
-        <v>2721</v>
       </c>
       <c r="BM277" s="1" t="s">
         <v>113</v>
@@ -54916,13 +54846,13 @@
         <v>114</v>
       </c>
       <c r="BR277" s="1" t="s">
-        <v>2722</v>
+        <v>2721</v>
       </c>
       <c r="BS277" s="3">
         <v>35206</v>
       </c>
       <c r="BT277" s="1" t="s">
-        <v>2723</v>
+        <v>2722</v>
       </c>
       <c r="BU277" s="1" t="s">
         <v>117</v>
@@ -54943,13 +54873,14 @@
         <v>713</v>
       </c>
       <c r="CD277" s="1" t="s">
+        <v>2723</v>
+      </c>
+      <c r="CE277" s="1" t="s">
         <v>2724</v>
-      </c>
-      <c r="CE277" s="1" t="s">
-        <v>2725</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:CF277" xr:uid="{DFF611CE-CEEF-43AD-AE31-A5FFA192CD45}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>